<commit_message>
updated fungi data sumbission
</commit_message>
<xml_diff>
--- a/assets/resources/TEMPLATE_DataFields_Vouchers_Fungi.xlsx
+++ b/assets/resources/TEMPLATE_DataFields_Vouchers_Fungi.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://dbotanicgardens.sharepoint.com/sites/FieldWork/Shared Documents/General/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\richard.levy\Denver Botanic Gardens\FieldWork - General\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="15" documentId="13_ncr:1_{46D17477-F485-4F6F-BC97-02ECBD1C8B1B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{DA115B83-25A5-480C-B597-7877BDC1FA55}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FF43B9A-8FFE-4E44-8884-11C4098BA3E5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="1800" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="62">
   <si>
     <t>recordedby</t>
   </si>
@@ -93,9 +93,6 @@
     <t>taste</t>
   </si>
   <si>
-    <t>host</t>
-  </si>
-  <si>
     <t>context</t>
   </si>
   <si>
@@ -105,9 +102,6 @@
     <t>stipe</t>
   </si>
   <si>
-    <t>tissue</t>
-  </si>
-  <si>
     <t>Primary Collector</t>
   </si>
   <si>
@@ -129,30 +123,15 @@
     <t>Identification Date</t>
   </si>
   <si>
-    <t>Y or N</t>
-  </si>
-  <si>
     <t>County Name Only</t>
   </si>
   <si>
-    <t>WGS84/NAD83/etc</t>
-  </si>
-  <si>
-    <t>vlaue for elevation in meters only</t>
-  </si>
-  <si>
-    <t>must write "feet" or "ft"</t>
-  </si>
-  <si>
     <t>associatedTaxa</t>
   </si>
   <si>
     <t>Latin binomials only|Only genus OK</t>
   </si>
   <si>
-    <t>occurrenceRemarks</t>
-  </si>
-  <si>
     <t>notes not otherwise captured</t>
   </si>
   <si>
@@ -162,15 +141,9 @@
     <t>fieldNumber</t>
   </si>
   <si>
-    <t>Other identifying number assigned to specimen in the field, at fair, or foray</t>
-  </si>
-  <si>
     <t>catalogNumber</t>
   </si>
   <si>
-    <t>barcode</t>
-  </si>
-  <si>
     <t>othercatalogNumbers</t>
   </si>
   <si>
@@ -196,13 +169,55 @@
   </si>
   <si>
     <t>iNaturalist ID</t>
+  </si>
+  <si>
+    <t>substrate</t>
+  </si>
+  <si>
+    <t>notes</t>
+  </si>
+  <si>
+    <t>DBG-F-###### barcode</t>
+  </si>
+  <si>
+    <t>value for elevation in meters only</t>
+  </si>
+  <si>
+    <t>only if provided in feet, must write "feet" or "ft"</t>
+  </si>
+  <si>
+    <t>WGS84</t>
+  </si>
+  <si>
+    <t>8 digit number from iNat</t>
+  </si>
+  <si>
+    <t>Detailed description of location where specimen was collected</t>
+  </si>
+  <si>
+    <t>plants nearby</t>
+  </si>
+  <si>
+    <t>identificationQualifier</t>
+  </si>
+  <si>
+    <t>Ex: cf., aff. The determiner’s expression of uncertainty in their identification.</t>
+  </si>
+  <si>
+    <t>only if collected within municipality</t>
+  </si>
+  <si>
+    <t>Unique barcode value from field slip</t>
+  </si>
+  <si>
+    <t>Name of event, project, or foray</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -226,6 +241,20 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF2B2B2B"/>
+      <name val="Lato"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -235,7 +264,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -243,11 +272,21 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -256,8 +295,17 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -570,316 +618,1245 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AK26"/>
+  <dimension ref="A1:AL320"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="P1" workbookViewId="0">
-      <selection activeCell="AH3" sqref="AH3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.5703125" customWidth="1"/>
-    <col min="4" max="4" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="33.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="30.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.85546875" customWidth="1"/>
-    <col min="7" max="7" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="30.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="43.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="57.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="6.28515625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="12" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="7.42578125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="17" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="31.5703125" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="22.7109375" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="7.28515625" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="4.85546875" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="33.28515625" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="27.7109375" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="5.5703125" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="6.42578125" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="5.140625" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="5.42578125" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="5.42578125" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="58" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.5703125" customWidth="1"/>
+    <col min="14" max="14" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="27.7109375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="5.140625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="5.42578125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="21.140625" style="13" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="43.42578125" style="10" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="70.7109375" style="10" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="57.7109375" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="5.42578125" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="6" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="21.5703125" style="13" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="12" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="31.5703125" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="45.28515625" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="33.28515625" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="40.85546875" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="17" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:37" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:38" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="K1" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="M1" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="R1" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="S1" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="T1" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="U1" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="AB1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="AC1" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="AD1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="AE1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="AF1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="AG1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="AH1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="AI1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="AJ1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="AK1" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="AL1" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="L1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:38" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="M1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="U1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="V1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="W1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="X1" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="Y1" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="Z1" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="AA1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="AB1" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="AC1" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="AD1" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="AE1" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="AF1" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="AG1" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="AH1" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="AI1" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="AJ1" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="AK1" s="5" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="2" spans="1:37" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="D2" s="2" t="s">
+      <c r="F2" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="E2" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>45</v>
-      </c>
       <c r="G2" s="2" t="s">
-        <v>29</v>
+        <v>42</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="K2" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="L2" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="N2" s="2" t="s">
-        <v>51</v>
-      </c>
+        <v>55</v>
+      </c>
+      <c r="K2" s="9"/>
+      <c r="M2" s="7"/>
       <c r="O2" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="T2" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="U2" s="2" t="s">
-        <v>37</v>
+      <c r="R2" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="S2" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="T2" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="U2" s="9" t="s">
+        <v>58</v>
       </c>
       <c r="V2" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="Y2" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="W2" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="AC2" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="Z2" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="AI2" s="7"/>
-      <c r="AJ2" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="AK2" s="6" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="3" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="G3" s="3"/>
-      <c r="K3" s="3"/>
-    </row>
-    <row r="4" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="G4" s="3"/>
-    </row>
-    <row r="5" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="G5" s="3"/>
-      <c r="K5" s="3"/>
-    </row>
-    <row r="6" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="G6" s="3"/>
-      <c r="K6" s="3"/>
-    </row>
-    <row r="7" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="G7" s="3"/>
-      <c r="K7" s="3"/>
-    </row>
-    <row r="8" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="G8" s="3"/>
-      <c r="K8" s="3"/>
-    </row>
-    <row r="9" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="G9" s="3"/>
-    </row>
-    <row r="10" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="G10" s="3"/>
-      <c r="K10" s="3"/>
-    </row>
-    <row r="11" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="G11" s="3"/>
-      <c r="K11" s="3"/>
-    </row>
-    <row r="12" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="G12" s="3"/>
-      <c r="K12" s="3"/>
-    </row>
-    <row r="13" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="G13" s="3"/>
-      <c r="K13" s="3"/>
-    </row>
-    <row r="14" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="G14" s="3"/>
-    </row>
-    <row r="15" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="G15" s="3"/>
-      <c r="K15" s="3"/>
-    </row>
-    <row r="16" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="G16" s="3"/>
-    </row>
-    <row r="17" spans="7:11" x14ac:dyDescent="0.25">
-      <c r="G17" s="3"/>
-      <c r="K17" s="3"/>
-    </row>
-    <row r="18" spans="7:11" x14ac:dyDescent="0.25">
-      <c r="G18" s="3"/>
-      <c r="K18" s="3"/>
-    </row>
-    <row r="19" spans="7:11" x14ac:dyDescent="0.25">
-      <c r="G19" s="3"/>
-      <c r="K19" s="3"/>
-    </row>
-    <row r="20" spans="7:11" x14ac:dyDescent="0.25">
-      <c r="G20" s="3"/>
-      <c r="K20" s="3"/>
-    </row>
-    <row r="21" spans="7:11" x14ac:dyDescent="0.25">
-      <c r="G21" s="3"/>
-      <c r="K21" s="3"/>
-    </row>
-    <row r="22" spans="7:11" x14ac:dyDescent="0.25">
-      <c r="G22" s="3"/>
-      <c r="K22" s="3"/>
-    </row>
-    <row r="23" spans="7:11" x14ac:dyDescent="0.25">
-      <c r="G23" s="3"/>
-      <c r="K23" s="3"/>
-    </row>
-    <row r="24" spans="7:11" x14ac:dyDescent="0.25">
-      <c r="G24" s="3"/>
-      <c r="K24" s="3"/>
-    </row>
-    <row r="25" spans="7:11" x14ac:dyDescent="0.25">
-      <c r="G25" s="3"/>
-      <c r="K25" s="3"/>
-    </row>
-    <row r="26" spans="7:11" x14ac:dyDescent="0.25">
-      <c r="G26" s="3"/>
+      <c r="AE2" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="AF2" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="AG2" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="AH2" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="AJ2" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="AK2" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="AL2" s="6" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="3" spans="1:38" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="F3" s="3"/>
+      <c r="K3" s="10"/>
+      <c r="U3" s="15"/>
+      <c r="V3" s="14"/>
+      <c r="W3" s="3"/>
+    </row>
+    <row r="4" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="F4" s="3"/>
+      <c r="K4" s="10"/>
+    </row>
+    <row r="5" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="F5" s="3"/>
+      <c r="K5" s="10"/>
+      <c r="W5" s="3"/>
+    </row>
+    <row r="6" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="F6" s="3"/>
+      <c r="K6" s="10"/>
+      <c r="W6" s="3"/>
+    </row>
+    <row r="7" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="F7" s="3"/>
+      <c r="K7" s="10"/>
+      <c r="W7" s="3"/>
+    </row>
+    <row r="8" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="F8" s="3"/>
+      <c r="K8" s="10"/>
+      <c r="W8" s="3"/>
+    </row>
+    <row r="9" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="F9" s="3"/>
+      <c r="K9" s="10"/>
+    </row>
+    <row r="10" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="F10" s="3"/>
+      <c r="K10" s="10"/>
+      <c r="W10" s="3"/>
+    </row>
+    <row r="11" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="F11" s="3"/>
+      <c r="K11" s="10"/>
+      <c r="W11" s="3"/>
+    </row>
+    <row r="12" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="F12" s="3"/>
+      <c r="K12" s="10"/>
+      <c r="W12" s="3"/>
+    </row>
+    <row r="13" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="F13" s="3"/>
+      <c r="K13" s="10"/>
+      <c r="W13" s="3"/>
+    </row>
+    <row r="14" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="F14" s="3"/>
+      <c r="K14" s="10"/>
+    </row>
+    <row r="15" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="F15" s="3"/>
+      <c r="K15" s="10"/>
+      <c r="W15" s="3"/>
+    </row>
+    <row r="16" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="F16" s="3"/>
+      <c r="K16" s="10"/>
+    </row>
+    <row r="17" spans="6:23" x14ac:dyDescent="0.25">
+      <c r="F17" s="3"/>
+      <c r="K17" s="10"/>
+      <c r="W17" s="3"/>
+    </row>
+    <row r="18" spans="6:23" x14ac:dyDescent="0.25">
+      <c r="F18" s="3"/>
+      <c r="K18" s="10"/>
+      <c r="W18" s="3"/>
+    </row>
+    <row r="19" spans="6:23" x14ac:dyDescent="0.25">
+      <c r="F19" s="3"/>
+      <c r="K19" s="10"/>
+      <c r="W19" s="3"/>
+    </row>
+    <row r="20" spans="6:23" x14ac:dyDescent="0.25">
+      <c r="F20" s="3"/>
+      <c r="K20" s="10"/>
+      <c r="W20" s="3"/>
+    </row>
+    <row r="21" spans="6:23" x14ac:dyDescent="0.25">
+      <c r="F21" s="3"/>
+      <c r="K21" s="10"/>
+      <c r="W21" s="3"/>
+    </row>
+    <row r="22" spans="6:23" x14ac:dyDescent="0.25">
+      <c r="F22" s="3"/>
+      <c r="K22" s="10"/>
+      <c r="W22" s="3"/>
+    </row>
+    <row r="23" spans="6:23" x14ac:dyDescent="0.25">
+      <c r="F23" s="3"/>
+      <c r="K23" s="10"/>
+      <c r="W23" s="3"/>
+    </row>
+    <row r="24" spans="6:23" x14ac:dyDescent="0.25">
+      <c r="F24" s="3"/>
+      <c r="K24" s="10"/>
+      <c r="W24" s="3"/>
+    </row>
+    <row r="25" spans="6:23" x14ac:dyDescent="0.25">
+      <c r="F25" s="3"/>
+      <c r="K25" s="10"/>
+      <c r="W25" s="3"/>
+    </row>
+    <row r="26" spans="6:23" x14ac:dyDescent="0.25">
+      <c r="F26" s="3"/>
+      <c r="K26" s="10"/>
+    </row>
+    <row r="27" spans="6:23" x14ac:dyDescent="0.25">
+      <c r="K27" s="10"/>
+    </row>
+    <row r="28" spans="6:23" x14ac:dyDescent="0.25">
+      <c r="K28" s="10"/>
+    </row>
+    <row r="29" spans="6:23" x14ac:dyDescent="0.25">
+      <c r="K29" s="10"/>
+    </row>
+    <row r="30" spans="6:23" x14ac:dyDescent="0.25">
+      <c r="K30" s="10"/>
+    </row>
+    <row r="31" spans="6:23" x14ac:dyDescent="0.25">
+      <c r="K31" s="10"/>
+    </row>
+    <row r="32" spans="6:23" x14ac:dyDescent="0.25">
+      <c r="K32" s="10"/>
+    </row>
+    <row r="33" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K33" s="10"/>
+    </row>
+    <row r="34" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K34" s="10"/>
+    </row>
+    <row r="35" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K35" s="10"/>
+    </row>
+    <row r="36" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K36" s="10"/>
+    </row>
+    <row r="37" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K37" s="10"/>
+    </row>
+    <row r="38" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K38" s="10"/>
+    </row>
+    <row r="39" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K39" s="10"/>
+    </row>
+    <row r="40" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K40" s="10"/>
+    </row>
+    <row r="41" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K41" s="10"/>
+    </row>
+    <row r="42" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K42" s="10"/>
+    </row>
+    <row r="43" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K43" s="10"/>
+    </row>
+    <row r="44" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K44" s="10"/>
+    </row>
+    <row r="45" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K45" s="10"/>
+    </row>
+    <row r="46" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K46" s="10"/>
+    </row>
+    <row r="47" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K47" s="10"/>
+    </row>
+    <row r="48" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K48" s="10"/>
+    </row>
+    <row r="49" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K49" s="10"/>
+    </row>
+    <row r="50" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K50" s="10"/>
+    </row>
+    <row r="51" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K51" s="10"/>
+    </row>
+    <row r="52" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K52" s="10"/>
+    </row>
+    <row r="53" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K53" s="10"/>
+    </row>
+    <row r="54" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K54" s="10"/>
+    </row>
+    <row r="55" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K55" s="10"/>
+    </row>
+    <row r="56" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K56" s="10"/>
+    </row>
+    <row r="57" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K57" s="10"/>
+    </row>
+    <row r="58" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K58" s="10"/>
+    </row>
+    <row r="59" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K59" s="10"/>
+    </row>
+    <row r="60" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K60" s="10"/>
+    </row>
+    <row r="61" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K61" s="10"/>
+    </row>
+    <row r="62" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K62" s="10"/>
+    </row>
+    <row r="63" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K63" s="10"/>
+    </row>
+    <row r="64" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K64" s="10"/>
+    </row>
+    <row r="65" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K65" s="10"/>
+    </row>
+    <row r="66" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K66" s="10"/>
+    </row>
+    <row r="67" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K67" s="10"/>
+    </row>
+    <row r="68" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K68" s="10"/>
+    </row>
+    <row r="69" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K69" s="10"/>
+    </row>
+    <row r="70" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K70" s="10"/>
+    </row>
+    <row r="71" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K71" s="10"/>
+    </row>
+    <row r="72" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K72" s="10"/>
+    </row>
+    <row r="73" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K73" s="10"/>
+    </row>
+    <row r="74" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K74" s="10"/>
+    </row>
+    <row r="75" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K75" s="10"/>
+    </row>
+    <row r="76" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K76" s="10"/>
+    </row>
+    <row r="77" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K77" s="10"/>
+    </row>
+    <row r="78" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K78" s="10"/>
+    </row>
+    <row r="79" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K79" s="10"/>
+    </row>
+    <row r="80" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K80" s="10"/>
+    </row>
+    <row r="81" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K81" s="10"/>
+    </row>
+    <row r="82" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K82" s="10"/>
+    </row>
+    <row r="83" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K83" s="10"/>
+    </row>
+    <row r="84" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K84" s="10"/>
+    </row>
+    <row r="85" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K85" s="10"/>
+    </row>
+    <row r="86" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K86" s="10"/>
+    </row>
+    <row r="87" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K87" s="10"/>
+    </row>
+    <row r="88" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K88" s="10"/>
+    </row>
+    <row r="89" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K89" s="10"/>
+    </row>
+    <row r="90" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K90" s="10"/>
+    </row>
+    <row r="91" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K91" s="10"/>
+    </row>
+    <row r="92" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K92" s="10"/>
+    </row>
+    <row r="93" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K93" s="10"/>
+    </row>
+    <row r="94" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K94" s="10"/>
+    </row>
+    <row r="95" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K95" s="10"/>
+    </row>
+    <row r="96" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K96" s="10"/>
+    </row>
+    <row r="97" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K97" s="10"/>
+    </row>
+    <row r="98" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K98" s="10"/>
+    </row>
+    <row r="99" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K99" s="10"/>
+    </row>
+    <row r="100" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K100" s="10"/>
+    </row>
+    <row r="101" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K101" s="10"/>
+    </row>
+    <row r="102" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K102" s="10"/>
+    </row>
+    <row r="103" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K103" s="10"/>
+    </row>
+    <row r="104" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K104" s="10"/>
+    </row>
+    <row r="105" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K105" s="10"/>
+    </row>
+    <row r="106" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K106" s="10"/>
+    </row>
+    <row r="107" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K107" s="10"/>
+    </row>
+    <row r="108" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K108" s="10"/>
+    </row>
+    <row r="109" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K109" s="10"/>
+    </row>
+    <row r="110" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K110" s="10"/>
+    </row>
+    <row r="111" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K111" s="10"/>
+    </row>
+    <row r="112" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K112" s="10"/>
+    </row>
+    <row r="113" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K113" s="10"/>
+    </row>
+    <row r="114" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K114" s="10"/>
+    </row>
+    <row r="115" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K115" s="10"/>
+    </row>
+    <row r="116" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K116" s="10"/>
+    </row>
+    <row r="117" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K117" s="10"/>
+    </row>
+    <row r="118" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K118" s="10"/>
+    </row>
+    <row r="119" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K119" s="10"/>
+    </row>
+    <row r="120" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K120" s="10"/>
+    </row>
+    <row r="121" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K121" s="10"/>
+    </row>
+    <row r="122" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K122" s="10"/>
+    </row>
+    <row r="123" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K123" s="10"/>
+    </row>
+    <row r="124" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K124" s="10"/>
+    </row>
+    <row r="125" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K125" s="10"/>
+    </row>
+    <row r="126" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K126" s="10"/>
+    </row>
+    <row r="127" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K127" s="10"/>
+    </row>
+    <row r="128" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K128" s="10"/>
+    </row>
+    <row r="129" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K129" s="10"/>
+    </row>
+    <row r="130" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K130" s="10"/>
+    </row>
+    <row r="131" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K131" s="10"/>
+    </row>
+    <row r="132" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K132" s="10"/>
+    </row>
+    <row r="133" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K133" s="10"/>
+    </row>
+    <row r="134" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K134" s="10"/>
+    </row>
+    <row r="135" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K135" s="10"/>
+    </row>
+    <row r="136" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K136" s="10"/>
+    </row>
+    <row r="137" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K137" s="10"/>
+    </row>
+    <row r="138" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K138" s="10"/>
+    </row>
+    <row r="139" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K139" s="10"/>
+    </row>
+    <row r="140" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K140" s="10"/>
+    </row>
+    <row r="141" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K141" s="10"/>
+    </row>
+    <row r="142" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K142" s="10"/>
+    </row>
+    <row r="143" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K143" s="10"/>
+    </row>
+    <row r="144" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K144" s="10"/>
+    </row>
+    <row r="145" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K145" s="10"/>
+    </row>
+    <row r="146" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K146" s="10"/>
+    </row>
+    <row r="147" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K147" s="10"/>
+    </row>
+    <row r="148" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K148" s="10"/>
+    </row>
+    <row r="149" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K149" s="10"/>
+    </row>
+    <row r="150" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K150" s="10"/>
+    </row>
+    <row r="151" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K151" s="10"/>
+    </row>
+    <row r="152" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K152" s="10"/>
+    </row>
+    <row r="153" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K153" s="10"/>
+    </row>
+    <row r="154" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K154" s="10"/>
+    </row>
+    <row r="155" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K155" s="10"/>
+    </row>
+    <row r="156" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K156" s="10"/>
+    </row>
+    <row r="157" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K157" s="10"/>
+    </row>
+    <row r="158" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K158" s="10"/>
+    </row>
+    <row r="159" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K159" s="10"/>
+    </row>
+    <row r="160" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K160" s="10"/>
+    </row>
+    <row r="161" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K161" s="10"/>
+    </row>
+    <row r="162" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K162" s="10"/>
+    </row>
+    <row r="163" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K163" s="10"/>
+    </row>
+    <row r="164" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K164" s="10"/>
+    </row>
+    <row r="165" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K165" s="10"/>
+    </row>
+    <row r="166" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K166" s="10"/>
+    </row>
+    <row r="167" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K167" s="10"/>
+    </row>
+    <row r="168" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K168" s="10"/>
+    </row>
+    <row r="169" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K169" s="10"/>
+    </row>
+    <row r="170" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K170" s="10"/>
+    </row>
+    <row r="171" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K171" s="10"/>
+    </row>
+    <row r="172" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K172" s="10"/>
+    </row>
+    <row r="173" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K173" s="10"/>
+    </row>
+    <row r="174" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K174" s="10"/>
+    </row>
+    <row r="175" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K175" s="10"/>
+    </row>
+    <row r="176" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K176" s="10"/>
+    </row>
+    <row r="177" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K177" s="10"/>
+    </row>
+    <row r="178" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K178" s="10"/>
+    </row>
+    <row r="179" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K179" s="10"/>
+    </row>
+    <row r="180" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K180" s="10"/>
+    </row>
+    <row r="181" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K181" s="10"/>
+    </row>
+    <row r="182" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K182" s="10"/>
+    </row>
+    <row r="183" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K183" s="10"/>
+    </row>
+    <row r="184" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K184" s="10"/>
+    </row>
+    <row r="185" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K185" s="10"/>
+    </row>
+    <row r="186" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K186" s="10"/>
+    </row>
+    <row r="187" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K187" s="10"/>
+    </row>
+    <row r="188" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K188" s="10"/>
+    </row>
+    <row r="189" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K189" s="10"/>
+    </row>
+    <row r="190" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K190" s="10"/>
+    </row>
+    <row r="191" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K191" s="10"/>
+    </row>
+    <row r="192" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K192" s="10"/>
+    </row>
+    <row r="193" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K193" s="10"/>
+    </row>
+    <row r="194" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K194" s="10"/>
+    </row>
+    <row r="195" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K195" s="10"/>
+    </row>
+    <row r="196" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K196" s="10"/>
+    </row>
+    <row r="197" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K197" s="10"/>
+    </row>
+    <row r="198" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K198" s="10"/>
+    </row>
+    <row r="199" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K199" s="10"/>
+    </row>
+    <row r="200" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K200" s="10"/>
+    </row>
+    <row r="201" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K201" s="10"/>
+    </row>
+    <row r="202" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K202" s="10"/>
+    </row>
+    <row r="203" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K203" s="10"/>
+    </row>
+    <row r="204" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K204" s="10"/>
+    </row>
+    <row r="205" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K205" s="10"/>
+    </row>
+    <row r="206" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K206" s="10"/>
+    </row>
+    <row r="207" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K207" s="10"/>
+    </row>
+    <row r="208" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K208" s="10"/>
+    </row>
+    <row r="209" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K209" s="10"/>
+    </row>
+    <row r="210" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K210" s="10"/>
+    </row>
+    <row r="211" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K211" s="10"/>
+    </row>
+    <row r="212" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K212" s="10"/>
+    </row>
+    <row r="213" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K213" s="10"/>
+    </row>
+    <row r="214" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K214" s="10"/>
+    </row>
+    <row r="215" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K215" s="10"/>
+    </row>
+    <row r="216" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K216" s="10"/>
+    </row>
+    <row r="217" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K217" s="10"/>
+    </row>
+    <row r="218" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K218" s="10"/>
+    </row>
+    <row r="219" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K219" s="10"/>
+    </row>
+    <row r="220" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K220" s="10"/>
+    </row>
+    <row r="221" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K221" s="10"/>
+    </row>
+    <row r="222" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K222" s="10"/>
+    </row>
+    <row r="223" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K223" s="10"/>
+    </row>
+    <row r="224" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K224" s="10"/>
+    </row>
+    <row r="225" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K225" s="10"/>
+    </row>
+    <row r="226" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K226" s="10"/>
+    </row>
+    <row r="227" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K227" s="10"/>
+    </row>
+    <row r="228" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K228" s="10"/>
+    </row>
+    <row r="229" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K229" s="10"/>
+    </row>
+    <row r="230" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K230" s="10"/>
+    </row>
+    <row r="231" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K231" s="10"/>
+    </row>
+    <row r="232" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K232" s="10"/>
+    </row>
+    <row r="233" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K233" s="10"/>
+    </row>
+    <row r="234" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K234" s="10"/>
+    </row>
+    <row r="235" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K235" s="10"/>
+    </row>
+    <row r="236" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K236" s="10"/>
+    </row>
+    <row r="237" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K237" s="10"/>
+    </row>
+    <row r="238" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K238" s="10"/>
+    </row>
+    <row r="239" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K239" s="10"/>
+    </row>
+    <row r="240" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K240" s="10"/>
+    </row>
+    <row r="241" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K241" s="10"/>
+    </row>
+    <row r="242" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K242" s="10"/>
+    </row>
+    <row r="243" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K243" s="10"/>
+    </row>
+    <row r="244" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K244" s="10"/>
+    </row>
+    <row r="245" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K245" s="10"/>
+    </row>
+    <row r="246" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K246" s="10"/>
+    </row>
+    <row r="247" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K247" s="10"/>
+    </row>
+    <row r="248" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K248" s="10"/>
+    </row>
+    <row r="249" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K249" s="10"/>
+    </row>
+    <row r="250" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K250" s="10"/>
+    </row>
+    <row r="251" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K251" s="10"/>
+    </row>
+    <row r="252" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K252" s="10"/>
+    </row>
+    <row r="253" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K253" s="10"/>
+    </row>
+    <row r="254" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K254" s="10"/>
+    </row>
+    <row r="255" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K255" s="10"/>
+    </row>
+    <row r="256" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K256" s="10"/>
+    </row>
+    <row r="257" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K257" s="10"/>
+    </row>
+    <row r="258" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K258" s="10"/>
+    </row>
+    <row r="259" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K259" s="10"/>
+    </row>
+    <row r="260" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K260" s="10"/>
+    </row>
+    <row r="261" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K261" s="10"/>
+    </row>
+    <row r="262" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K262" s="10"/>
+    </row>
+    <row r="263" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K263" s="10"/>
+    </row>
+    <row r="264" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K264" s="10"/>
+    </row>
+    <row r="265" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K265" s="10"/>
+    </row>
+    <row r="266" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K266" s="10"/>
+    </row>
+    <row r="267" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K267" s="10"/>
+    </row>
+    <row r="268" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K268" s="10"/>
+    </row>
+    <row r="269" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K269" s="10"/>
+    </row>
+    <row r="270" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K270" s="10"/>
+    </row>
+    <row r="271" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K271" s="10"/>
+    </row>
+    <row r="272" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K272" s="10"/>
+    </row>
+    <row r="273" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K273" s="10"/>
+    </row>
+    <row r="274" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K274" s="10"/>
+    </row>
+    <row r="275" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K275" s="10"/>
+    </row>
+    <row r="276" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K276" s="10"/>
+    </row>
+    <row r="277" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K277" s="10"/>
+    </row>
+    <row r="278" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K278" s="10"/>
+    </row>
+    <row r="279" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K279" s="10"/>
+    </row>
+    <row r="280" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K280" s="10"/>
+    </row>
+    <row r="281" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K281" s="10"/>
+    </row>
+    <row r="282" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K282" s="10"/>
+    </row>
+    <row r="283" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K283" s="10"/>
+    </row>
+    <row r="284" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K284" s="10"/>
+    </row>
+    <row r="285" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K285" s="10"/>
+    </row>
+    <row r="286" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K286" s="10"/>
+    </row>
+    <row r="287" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K287" s="10"/>
+    </row>
+    <row r="288" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K288" s="10"/>
+    </row>
+    <row r="289" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K289" s="10"/>
+    </row>
+    <row r="290" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K290" s="10"/>
+    </row>
+    <row r="291" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K291" s="10"/>
+    </row>
+    <row r="292" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K292" s="10"/>
+    </row>
+    <row r="293" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K293" s="10"/>
+    </row>
+    <row r="294" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K294" s="10"/>
+    </row>
+    <row r="295" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K295" s="10"/>
+    </row>
+    <row r="296" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K296" s="10"/>
+    </row>
+    <row r="297" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K297" s="10"/>
+    </row>
+    <row r="298" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K298" s="10"/>
+    </row>
+    <row r="299" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K299" s="10"/>
+    </row>
+    <row r="300" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K300" s="10"/>
+    </row>
+    <row r="301" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K301" s="10"/>
+    </row>
+    <row r="302" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K302" s="10"/>
+    </row>
+    <row r="303" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K303" s="10"/>
+    </row>
+    <row r="304" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K304" s="10"/>
+    </row>
+    <row r="305" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K305" s="10"/>
+    </row>
+    <row r="306" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K306" s="10"/>
+    </row>
+    <row r="307" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K307" s="10"/>
+    </row>
+    <row r="308" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K308" s="10"/>
+    </row>
+    <row r="309" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K309" s="10"/>
+    </row>
+    <row r="310" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K310" s="10"/>
+    </row>
+    <row r="311" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K311" s="10"/>
+    </row>
+    <row r="312" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K312" s="10"/>
+    </row>
+    <row r="313" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K313" s="10"/>
+    </row>
+    <row r="314" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K314" s="10"/>
+    </row>
+    <row r="315" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K315" s="10"/>
+    </row>
+    <row r="316" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K316" s="10"/>
+    </row>
+    <row r="317" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K317" s="10"/>
+    </row>
+    <row r="318" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K318" s="10"/>
+    </row>
+    <row r="319" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K319" s="10"/>
+    </row>
+    <row r="320" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K320" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -888,21 +1865,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D1BE5CD796B69543BA7FCF39B9A430F9" ma:contentTypeVersion="10" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="48f98be3a9b998f19577fe96e9026a80">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="bf26cdc5-6581-43e5-a643-41a56d0810f3" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="73b90b828ce3bab7196225ca911adf86" ns2:_="">
     <xsd:import namespace="bf26cdc5-6581-43e5-a643-41a56d0810f3"/>
@@ -1086,24 +2048,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D8421DEF-4AC9-4971-B328-F90C65F8D037}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BFB4E40D-EAB7-4B9D-ACA8-A99E849A9F1C}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{723B0D33-11F7-4F74-AA58-4AA22D4BF2EF}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1119,4 +2079,21 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D8421DEF-4AC9-4971-B328-F90C65F8D037}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BFB4E40D-EAB7-4B9D-ACA8-A99E849A9F1C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>